<commit_message>
Test cases for bootstrap- additional changes CCA field done.
</commit_message>
<xml_diff>
--- a/testing/iteration 5/OFFICIAL Testing - Iter 5.xlsx
+++ b/testing/iteration 5/OFFICIAL Testing - Iter 5.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="131">
   <si>
     <t>TEST CASES</t>
   </si>
@@ -406,6 +406,15 @@
   </si>
   <si>
     <t>BASIC-APP.ZIP</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Load the zip file</t>
+  </si>
+  <si>
+    <t>"invalid header"</t>
   </si>
 </sst>
 </file>
@@ -2229,8 +2238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2239,7 +2248,8 @@
     <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -2268,7 +2278,7 @@
       <c r="G2" s="50"/>
       <c r="H2" s="51"/>
     </row>
-    <row r="3" spans="1:8" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -2307,6 +2317,12 @@
       <c r="D4" t="s">
         <v>102</v>
       </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -2321,6 +2337,12 @@
       <c r="D5" t="s">
         <v>106</v>
       </c>
+      <c r="E5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -2335,6 +2357,12 @@
       <c r="D6" t="s">
         <v>107</v>
       </c>
+      <c r="E6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -2349,13 +2377,19 @@
       <c r="D7" t="s">
         <v>108</v>
       </c>
+      <c r="E7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C8" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
Completed updating test case and done testing for BASIC APP- Breakdown by usage time category and demographics
</commit_message>
<xml_diff>
--- a/testing/iteration 5/OFFICIAL Testing - Iter 5.xlsx
+++ b/testing/iteration 5/OFFICIAL Testing - Iter 5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="320" windowWidth="19140" windowHeight="8340" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="380" windowWidth="19140" windowHeight="8280" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TOPK" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="154">
   <si>
     <t>TEST CASES</t>
   </si>
@@ -415,6 +415,75 @@
   </si>
   <si>
     <t>"invalid header"</t>
+  </si>
+  <si>
+    <t>Input start and end date as 6April 2015, select filter as gender</t>
+  </si>
+  <si>
+    <t>User are able to sort by Gender accurately</t>
+  </si>
+  <si>
+    <t>50% Female, 50% Male, both mild</t>
+  </si>
+  <si>
+    <t>User are able to sort by School accurately</t>
+  </si>
+  <si>
+    <t>Input start and end date as 6April 2015, select filter as School</t>
+  </si>
+  <si>
+    <t>1 mild user from econs, 1 from accountancy and 2 from sosci</t>
+  </si>
+  <si>
+    <t>User are able to sort by Year accurately</t>
+  </si>
+  <si>
+    <t>Input start and end date as 6April 2015, select filter as Year</t>
+  </si>
+  <si>
+    <t>1 from 2015, 2 from 2014, 1 from 2012</t>
+  </si>
+  <si>
+    <t>Test if the calculation of Intense, Moderate and Mild work</t>
+  </si>
+  <si>
+    <t>Try out all filter</t>
+  </si>
+  <si>
+    <t>Test the filters, if I can randomly select a filter if I only have 1 demographics to sort out in mind</t>
+  </si>
+  <si>
+    <t>All filters can work</t>
+  </si>
+  <si>
+    <t>Input start and end date as 6April 2015, select filter as CCA</t>
+  </si>
+  <si>
+    <t>Test if the average function work</t>
+  </si>
+  <si>
+    <t>BASIC-APP2.ZIP</t>
+  </si>
+  <si>
+    <t>75% choir, 25% soccer</t>
+  </si>
+  <si>
+    <t>Result of all fields should be similar to row 2-4</t>
+  </si>
+  <si>
+    <t>Result of all fields same as what row 2-4 returns</t>
+  </si>
+  <si>
+    <t>Retry row 2-4, but this time date is 06/04/2015 to 07/04/2015</t>
+  </si>
+  <si>
+    <t>BASIC-APP3.ZIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50% Female both mild, 50% Male with one normal and one mild </t>
+  </si>
+  <si>
+    <t>"value must be 01/01/1970 and later"</t>
   </si>
 </sst>
 </file>
@@ -667,7 +736,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -769,6 +838,12 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1120,16 +1195,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="51"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:8" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -1403,11 +1478,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="56"/>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
@@ -1455,11 +1530,11 @@
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="54"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="56"/>
       <c r="D8" s="26"/>
     </row>
     <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1520,11 +1595,11 @@
     </row>
     <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="54"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
     </row>
     <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="23" t="s">
@@ -1573,11 +1648,11 @@
     </row>
     <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="54"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="56"/>
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="23" t="s">
@@ -1617,7 +1692,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:H3"/>
+      <selection activeCell="C4" sqref="C4:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1648,16 +1723,16 @@
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="51"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -1870,11 +1945,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="56"/>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="46" t="s">
@@ -1963,11 +2038,11 @@
       <c r="C11" s="28"/>
     </row>
     <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="56"/>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="46" t="s">
@@ -2045,11 +2120,11 @@
       <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="52" t="s">
+      <c r="A22" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="53"/>
-      <c r="C22" s="54"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="56"/>
     </row>
     <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="46" t="s">
@@ -2136,11 +2211,11 @@
       <c r="C32" s="6"/>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="52" t="s">
+      <c r="A33" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="B33" s="53"/>
-      <c r="C33" s="54"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="56"/>
     </row>
     <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="46" t="s">
@@ -2238,7 +2313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -2267,16 +2342,16 @@
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="51"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -2463,16 +2538,16 @@
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="51"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -2600,10 +2675,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2611,6 +2686,8 @@
     <col min="2" max="2" width="35.36328125" customWidth="1"/>
     <col min="3" max="3" width="42.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -2630,16 +2707,16 @@
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="51"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -2667,7 +2744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2678,7 +2755,253 @@
         <v>122</v>
       </c>
       <c r="D4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" t="s">
         <v>127</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="G8" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="H8" s="50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="145" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H9" s="50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="G10" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="H10" s="50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H11" s="50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H12" s="50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="50" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed test cases for basic app for all 4 parts.
</commit_message>
<xml_diff>
--- a/testing/iteration 5/OFFICIAL Testing - Iter 5.xlsx
+++ b/testing/iteration 5/OFFICIAL Testing - Iter 5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="380" windowWidth="19140" windowHeight="8280" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="19140" windowHeight="8220" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TOPK" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="177">
   <si>
     <t>TEST CASES</t>
   </si>
@@ -484,6 +484,75 @@
   </si>
   <si>
     <t>"value must be 01/01/1970 and later"</t>
+  </si>
+  <si>
+    <t>Breakdown by app category</t>
+  </si>
+  <si>
+    <t>BASIC-APP4.ZIP</t>
+  </si>
+  <si>
+    <t>The breakdown array is sorted by category name ascending.</t>
+  </si>
+  <si>
+    <t>Check correct percentage calculation by category</t>
+  </si>
+  <si>
+    <t>16 for books and 71 for social</t>
+  </si>
+  <si>
+    <t>Check for correct duration per category of appusage by category</t>
+  </si>
+  <si>
+    <t>82% social and 18% books</t>
+  </si>
+  <si>
+    <t>Result sorted in category ascending order</t>
+  </si>
+  <si>
+    <t>Diurnal pattern of app usage time</t>
+  </si>
+  <si>
+    <t>Check for correct result per timing</t>
+  </si>
+  <si>
+    <t>BASIC-APP5.ZIP</t>
+  </si>
+  <si>
+    <t>Start date is 06/04/2015 , end date is 06/04/2015, filter by Year and choose year 2015</t>
+  </si>
+  <si>
+    <t>BASIC-APP6.ZIP</t>
+  </si>
+  <si>
+    <t>Start date is 06/04/2015 , end date is 07/04/2015, filter by Gender and choose Female and filter by year choose 2012</t>
+  </si>
+  <si>
+    <t>13:00-14:00 is total of 21seconds , 16:00 to 17:00 is a total of 60 sec, 17:00 to 18:00 is 70 seconds, the rest 0</t>
+  </si>
+  <si>
+    <t>13:00-14:00 is a total of 156 secs, time 14:00 to 17:00 would have a daily 130 secs PER HOUR, and 18:00 to 19:00 would have 3480 seconds, the rest 0</t>
+  </si>
+  <si>
+    <t>Check for the handling of 16:59:00 to 17:01:00  (next timing) record and multiple demographics selection</t>
+  </si>
+  <si>
+    <t>Check of valid date</t>
+  </si>
+  <si>
+    <t>sets start as 4-12-0001</t>
+  </si>
+  <si>
+    <t>Check for more than one demographics, select by Gender then by CCA</t>
+  </si>
+  <si>
+    <t>Display male, followed by choir 1 with 1 mild user. And soccer with 1 mild user. For female, we have 2 choir with mile user, soccer will be 0.</t>
+  </si>
+  <si>
+    <t>Display male, followed by choir 1 with 1 mild user. And soccer with 1 mild user. For female, we have 2 choir with mile user, soccer will be  0</t>
+  </si>
+  <si>
+    <t>Pass, but do you think we need to display the 0 record for soccer?</t>
   </si>
 </sst>
 </file>
@@ -2511,8 +2580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2675,19 +2744,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="35.36328125" customWidth="1"/>
-    <col min="3" max="3" width="42.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -3004,6 +3074,255 @@
         <v>35</v>
       </c>
     </row>
+    <row r="14" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="H14" s="50" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" t="s">
+        <v>158</v>
+      </c>
+      <c r="G15" t="s">
+        <v>158</v>
+      </c>
+      <c r="H15" s="50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G16" t="s">
+        <v>158</v>
+      </c>
+      <c r="H16" s="50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" t="s">
+        <v>155</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H17" s="50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H18" s="50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H19" s="50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H21" s="50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D22" s="50" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:H2"/>
@@ -3012,5 +3331,6 @@
     <hyperlink ref="D1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated test cases for social activeness
</commit_message>
<xml_diff>
--- a/testing/iteration 5/OFFICIAL Testing - Iter 5.xlsx
+++ b/testing/iteration 5/OFFICIAL Testing - Iter 5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="19140" windowHeight="8220" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19140" windowHeight="8160" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TOPK" sheetId="1" r:id="rId1"/>
@@ -1761,7 +1761,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:F6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2002,8 +2002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="B40" s="40"/>
       <c r="C40" s="41">
-        <v>206</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -2355,7 +2355,7 @@
       </c>
       <c r="B41" s="40"/>
       <c r="C41" s="42">
-        <v>0.92718446601941751</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2364,7 +2364,7 @@
       </c>
       <c r="B42" s="44"/>
       <c r="C42" s="45">
-        <v>7.281553398058252E-2</v>
+        <v>0.61</v>
       </c>
     </row>
   </sheetData>
@@ -2746,7 +2746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
+    <sheetView topLeftCell="D18" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Organised test cases for iteration 5
</commit_message>
<xml_diff>
--- a/testing/iteration 5/OFFICIAL Testing - Iter 5.xlsx
+++ b/testing/iteration 5/OFFICIAL Testing - Iter 5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19140" windowHeight="8160" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="19140" windowHeight="7980" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TOPK" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="191">
   <si>
     <t>TEST CASES</t>
   </si>
@@ -113,19 +113,10 @@
     <t>Check for valid start date before end date</t>
   </si>
   <si>
-    <t>Nothing is displayed</t>
-  </si>
-  <si>
     <t>k=5, startdate 6 April, end date 8 April, school = soscs</t>
   </si>
   <si>
-    <t>2 Results, Rank 1 TouchWizHome and Rank 2 Taxi Booking is displayed</t>
-  </si>
-  <si>
     <t>Blank Page</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>Pass</t>
@@ -333,9 +324,6 @@
     <t>BOOTSTRAP-CHANGE1.ZIP</t>
   </si>
   <si>
-    <t>Read and handle CCA Functions properly</t>
-  </si>
-  <si>
     <t xml:space="preserve">Extra spaces before header </t>
   </si>
   <si>
@@ -387,9 +375,6 @@
     <t>CCA field validation(Length 70)</t>
   </si>
   <si>
-    <t xml:space="preserve"> “cca record too long”</t>
-  </si>
-  <si>
     <t>User are able to sort by CCA - Try selecting by CCA</t>
   </si>
   <si>
@@ -414,9 +399,6 @@
     <t>Load the zip file</t>
   </si>
   <si>
-    <t>"invalid header"</t>
-  </si>
-  <si>
     <t>Input start and end date as 6April 2015, select filter as gender</t>
   </si>
   <si>
@@ -528,12 +510,6 @@
     <t>Start date is 06/04/2015 , end date is 07/04/2015, filter by Gender and choose Female and filter by year choose 2012</t>
   </si>
   <si>
-    <t>13:00-14:00 is total of 21seconds , 16:00 to 17:00 is a total of 60 sec, 17:00 to 18:00 is 70 seconds, the rest 0</t>
-  </si>
-  <si>
-    <t>13:00-14:00 is a total of 156 secs, time 14:00 to 17:00 would have a daily 130 secs PER HOUR, and 18:00 to 19:00 would have 3480 seconds, the rest 0</t>
-  </si>
-  <si>
     <t>Check for the handling of 16:59:00 to 17:01:00  (next timing) record and multiple demographics selection</t>
   </si>
   <si>
@@ -555,17 +531,77 @@
     <t>Pass, but do you think we need to display the 0 record for soccer?</t>
   </si>
   <si>
-    <t>Try deleting by using this file</t>
-  </si>
-  <si>
-    <t>2 records deleted</t>
+    <t>Total Time Spent in SIS</t>
+  </si>
+  <si>
+    <t>Group Percent</t>
+  </si>
+  <si>
+    <t>Solo Percent</t>
+  </si>
+  <si>
+    <t>Correct Results</t>
+  </si>
+  <si>
+    <t>sets date as 4-12-0001</t>
+  </si>
+  <si>
+    <t>"invalid date"</t>
+  </si>
+  <si>
+    <t>Check of start date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correct </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> “cca record too long” IN ROW 2</t>
+  </si>
+  <si>
+    <t>Start date is 07/04/2015, filter by Gender and choose Female and filter by year choose 2014</t>
+  </si>
+  <si>
+    <t>16:00-17:00, 10 seconds, 17:00-18:00 10 seconds</t>
+  </si>
+  <si>
+    <t>13:00-14:00 is total of 21seconds , the rest 0</t>
+  </si>
+  <si>
+    <t>Try deleting by using this file(with location-del.csv)</t>
+  </si>
+  <si>
+    <t>1 records deleted</t>
+  </si>
+  <si>
+    <t>Upload DELLOC</t>
+  </si>
+  <si>
+    <t>13:00-14:00 is a total of 207 secs, time 14:00 to 17:00 would have a daily 130 secs PER HOUR, and 18:00 to 19:00 would have 3490 seconds, 19:00 to 20:00 10 seconds the rest 0</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>Try a location</t>
+  </si>
+  <si>
+    <t>Try a semantic place</t>
+  </si>
+  <si>
+    <t>Try both semantic place and location id</t>
+  </si>
+  <si>
+    <t>Try mac add</t>
+  </si>
+  <si>
+    <t>Try input dates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -631,8 +667,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -657,8 +699,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9F9F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -804,6 +852,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -811,7 +889,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -900,9 +978,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -918,6 +993,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1243,8 +1333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1270,16 +1360,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="55"/>
     </row>
     <row r="3" spans="1:8" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -1312,7 +1402,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -1324,10 +1414,10 @@
         <v>9</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -1335,7 +1425,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>
@@ -1347,10 +1437,10 @@
         <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1358,22 +1448,22 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1381,22 +1471,22 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1404,7 +1494,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>29</v>
@@ -1416,10 +1506,10 @@
         <v>16</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="116" x14ac:dyDescent="0.35">
@@ -1427,25 +1517,25 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>32</v>
+        <v>172</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1453,7 +1543,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>21</v>
@@ -1465,13 +1555,13 @@
         <v>24</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>172</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="58" customHeight="1" x14ac:dyDescent="0.35">
@@ -1479,7 +1569,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>22</v>
@@ -1491,13 +1581,13 @@
         <v>24</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>172</v>
       </c>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
@@ -1505,25 +1595,25 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>34</v>
+        <v>172</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1542,7 +1632,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1553,21 +1643,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="56"/>
+      <c r="A1" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1575,10 +1665,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C3" s="10">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1586,7 +1676,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C4" s="10">
         <v>11</v>
@@ -1597,7 +1687,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C5" s="13">
         <v>10</v>
@@ -1605,25 +1695,25 @@
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="56"/>
+      <c r="A8" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="57"/>
+      <c r="C8" s="58"/>
       <c r="D8" s="26"/>
     </row>
     <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -1631,13 +1721,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D10" s="19">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -1645,10 +1735,10 @@
         <v>2</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D11" s="19">
         <v>22</v>
@@ -1659,10 +1749,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D12" s="22">
         <v>10</v>
@@ -1670,21 +1760,21 @@
     </row>
     <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="56"/>
+      <c r="A14" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
     </row>
     <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -1692,11 +1782,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C16" s="19">
-        <f>SUM(45)</f>
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1704,7 +1793,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C17" s="19">
         <v>22</v>
@@ -1715,7 +1804,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C18" s="22">
         <v>10</v>
@@ -1723,21 +1812,21 @@
     </row>
     <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="55"/>
-      <c r="C20" s="56"/>
+      <c r="A20" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="57"/>
+      <c r="C20" s="58"/>
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1745,10 +1834,10 @@
         <v>1</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C22" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1764,10 +1853,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1792,22 +1881,22 @@
         <v>18</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="55"/>
     </row>
     <row r="3" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -1840,158 +1929,134 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="E5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="5">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="E6" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="5">
-        <v>4</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="E7" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>77</v>
+        <v>67</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
-      <c r="B9" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G9" s="1"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2006,10 +2071,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2019,377 +2084,329 @@
     <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="56"/>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" s="48" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="29" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="31">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="32" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C4" s="34">
         <v>0.11538461538461539</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="35"/>
       <c r="B5" s="33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C5" s="34">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F5" s="49"/>
+      <c r="G5" s="50"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="35"/>
       <c r="B6" s="33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C6" s="34">
         <v>0.38461538461538464</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F6" s="48"/>
+      <c r="G6" s="51"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="35"/>
       <c r="B7" s="33"/>
       <c r="C7" s="31"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="31">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="34">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="38">
-        <v>0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" s="37"/>
+      <c r="C8" s="38">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="37"/>
+      <c r="C9" s="39">
+        <v>0.62</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" s="41"/>
+      <c r="C10" s="42">
+        <v>0.38</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="27"/>
       <c r="B11" s="27"/>
       <c r="C11" s="28"/>
     </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="54" t="s">
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="57"/>
+      <c r="C12" s="58"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="55"/>
-      <c r="C12" s="56"/>
-    </row>
-    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" s="48" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="41">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" s="42">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="39">
         <v>0.1875</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="39"/>
-      <c r="B16" s="40" t="s">
-        <v>84</v>
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="40"/>
+      <c r="B16" s="41" t="s">
+        <v>81</v>
       </c>
       <c r="C16" s="42">
         <v>0.8125</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="39"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="41"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="39" t="s">
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="57"/>
+      <c r="C18" s="58"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="39">
+        <v>3.5294117647058823E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="36"/>
+      <c r="B22" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="39">
+        <v>0.15294117647058825</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="40"/>
+      <c r="B23" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="41">
+      <c r="C23" s="42">
+        <v>0.81176470588235294</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="57"/>
+      <c r="C25" s="58"/>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="37"/>
+      <c r="C27" s="38">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="39" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="39">
+        <v>0.11538461538461539</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="36"/>
+      <c r="B29" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="42">
-        <v>0.42307692307692307</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="45">
-        <v>0.57692307692307687</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" s="55"/>
-      <c r="C22" s="56"/>
-    </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="B23" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="C23" s="48" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="39" t="s">
+      <c r="C29" s="39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="36"/>
+      <c r="B30" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="39">
+        <v>0.38461538461538464</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="36"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="38"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="37"/>
+      <c r="C32" s="38">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="40"/>
-      <c r="C24" s="41">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="39" t="s">
+      <c r="B33" s="37"/>
+      <c r="C33" s="39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="42">
-        <v>3.5294117647058823E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="39"/>
-      <c r="B26" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="42">
-        <v>0.15294117647058825</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="39"/>
-      <c r="B27" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="42">
-        <v>0.81176470588235294</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="39"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="41"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="41">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="42">
-        <v>0.12941176470588237</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="44"/>
-      <c r="C31" s="45">
-        <v>0.87058823529411766</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C32" s="6"/>
-    </row>
-    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="B33" s="55"/>
-      <c r="C33" s="56"/>
-    </row>
-    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="B34" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34" s="48" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="B35" s="40"/>
-      <c r="C35" s="41">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="B36" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="42">
-        <v>0.11538461538461539</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="39"/>
-      <c r="B37" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="C37" s="42">
+      <c r="B34" s="41"/>
+      <c r="C34" s="42">
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="39"/>
-      <c r="B38" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="42">
-        <v>0.38461538461538464</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="39"/>
-      <c r="B39" s="40"/>
-      <c r="C39" s="41"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="40"/>
-      <c r="C40" s="41">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="42">
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B42" s="44"/>
-      <c r="C42" s="45">
-        <v>0.61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2417,16 +2434,16 @@
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="55"/>
     </row>
     <row r="3" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -2459,116 +2476,120 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" t="s">
         <v>124</v>
       </c>
-      <c r="C4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E4" t="s">
-        <v>129</v>
-      </c>
       <c r="F4" t="s">
-        <v>128</v>
+        <v>123</v>
+      </c>
+      <c r="G4" t="s">
+        <v>176</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" t="s">
         <v>124</v>
       </c>
-      <c r="C5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E5" t="s">
-        <v>129</v>
-      </c>
       <c r="F5" t="s">
-        <v>128</v>
+        <v>123</v>
+      </c>
+      <c r="G5" t="s">
+        <v>176</v>
+      </c>
+      <c r="H5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" t="s">
         <v>124</v>
       </c>
-      <c r="C6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E6" t="s">
-        <v>129</v>
-      </c>
       <c r="F6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+      <c r="G6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="C7" t="s">
         <v>105</v>
       </c>
       <c r="D7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
-      </c>
-      <c r="E8" t="s">
-        <v>111</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" t="s">
-        <v>121</v>
+        <v>104</v>
+      </c>
+      <c r="F8" t="s">
+        <v>177</v>
+      </c>
+      <c r="G8" t="s">
+        <v>176</v>
+      </c>
+      <c r="H8" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2586,8 +2607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2613,16 +2634,16 @@
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="55"/>
     </row>
     <row r="3" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -2655,13 +2676,25 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>120</v>
+      </c>
+      <c r="E4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4" t="s">
+        <v>185</v>
+      </c>
+      <c r="G4" t="s">
+        <v>185</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.35">
@@ -2669,16 +2702,25 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
-        <v>115</v>
+        <v>111</v>
+      </c>
+      <c r="F5" t="s">
+        <v>185</v>
+      </c>
+      <c r="G5" t="s">
+        <v>185</v>
+      </c>
+      <c r="H5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -2686,13 +2728,25 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>120</v>
+      </c>
+      <c r="E6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F6" t="s">
+        <v>185</v>
+      </c>
+      <c r="G6" t="s">
+        <v>185</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -2700,13 +2754,25 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D7" t="s">
-        <v>125</v>
+        <v>120</v>
+      </c>
+      <c r="E7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F7" t="s">
+        <v>185</v>
+      </c>
+      <c r="G7" t="s">
+        <v>185</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -2714,13 +2780,25 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D8" t="s">
-        <v>125</v>
+        <v>120</v>
+      </c>
+      <c r="E8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G8" t="s">
+        <v>185</v>
+      </c>
+      <c r="H8" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -2728,13 +2806,22 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>120</v>
+      </c>
+      <c r="E9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G9" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -2742,13 +2829,25 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>181</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" t="s">
+        <v>183</v>
       </c>
       <c r="F10" t="s">
-        <v>178</v>
+        <v>182</v>
+      </c>
+      <c r="G10" t="s">
+        <v>182</v>
+      </c>
+      <c r="H10" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2764,10 +2863,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="D18" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2791,22 +2890,22 @@
         <v>18</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="55"/>
     </row>
     <row r="3" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -2839,25 +2938,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="116" x14ac:dyDescent="0.35">
@@ -2865,25 +2964,25 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
@@ -2891,51 +2990,51 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -2943,77 +3042,77 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C8" s="49" t="s">
-        <v>142</v>
+        <v>118</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>136</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" s="50" t="s">
-        <v>141</v>
-      </c>
-      <c r="F8" s="50" t="s">
-        <v>143</v>
-      </c>
-      <c r="G8" s="50" t="s">
-        <v>143</v>
-      </c>
-      <c r="H8" s="50" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="145" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+      <c r="E8" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="G8" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="H8" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D9" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="H9" s="50" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+      <c r="H9" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
-      </c>
-      <c r="E10" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="F10" s="50" t="s">
-        <v>148</v>
-      </c>
-      <c r="G10" s="50" t="s">
-        <v>149</v>
-      </c>
-      <c r="H10" s="50" t="s">
-        <v>35</v>
+        <v>140</v>
+      </c>
+      <c r="E10" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="H10" s="47" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -3021,25 +3120,25 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H11" s="50" t="s">
-        <v>35</v>
+        <v>147</v>
+      </c>
+      <c r="H11" s="47" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -3047,25 +3146,25 @@
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H12" s="50" t="s">
-        <v>35</v>
+        <v>147</v>
+      </c>
+      <c r="H12" s="47" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -3073,7 +3172,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>29</v>
@@ -3082,7 +3181,7 @@
         <v>15</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>16</v>
@@ -3090,8 +3189,8 @@
       <c r="G13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="50" t="s">
-        <v>35</v>
+      <c r="H13" s="47" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
@@ -3099,25 +3198,25 @@
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="H14" s="50" t="s">
-        <v>176</v>
+        <v>167</v>
+      </c>
+      <c r="H14" s="47" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
@@ -3125,77 +3224,77 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D15" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F15" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="G15" t="s">
-        <v>158</v>
-      </c>
-      <c r="H15" s="50" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+      <c r="H15" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D16" t="s">
+        <v>149</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" t="s">
         <v>154</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D16" t="s">
-        <v>155</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" t="s">
-        <v>160</v>
-      </c>
       <c r="G16" t="s">
-        <v>158</v>
-      </c>
-      <c r="H16" s="50" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+      <c r="H16" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D17" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="G17" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="H17" s="50" t="s">
-        <v>35</v>
+        <v>155</v>
+      </c>
+      <c r="H17" s="47" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -3203,25 +3302,25 @@
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H18" s="50" t="s">
-        <v>35</v>
+        <v>147</v>
+      </c>
+      <c r="H18" s="47" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -3229,25 +3328,25 @@
         <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H19" s="50" t="s">
-        <v>35</v>
+        <v>147</v>
+      </c>
+      <c r="H19" s="47" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3255,7 +3354,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>29</v>
@@ -3264,7 +3363,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>16</v>
@@ -3272,8 +3371,8 @@
       <c r="G20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="50" t="s">
-        <v>35</v>
+      <c r="H20" s="47" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -3281,66 +3380,100 @@
         <v>18</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H21" s="50" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+      <c r="H21" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D22" s="50" t="s">
-        <v>165</v>
+        <v>157</v>
+      </c>
+      <c r="D22" s="47" t="s">
+        <v>159</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H22" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H23" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D23" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>168</v>
+      <c r="D24" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H24" s="47" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>